<commit_message>
updtae pages and others
</commit_message>
<xml_diff>
--- a/Burndown.xlsx
+++ b/Burndown.xlsx
@@ -8,17 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp12\htdocs\GL_PROJECT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FBAA77C1-2483-436D-8BEF-62F6070B86CC}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14A1A826-7F82-4258-8E7E-E62D13C0A7B3}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Burndown" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Burndown!$B$2:$B$4</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Burndown!$C$2:$C$4</definedName>
-  </definedNames>
   <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -231,16 +227,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="+mj-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
@@ -254,8 +250,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="1.4973071932599729E-3"/>
-          <c:y val="0.82926829268292679"/>
+          <c:x val="0.45161224807970413"/>
+          <c:y val="0.10108942368422275"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -271,16 +267,16 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="fr-FR"/>
@@ -318,31 +314,90 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="9525" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent1">
+                  <a:alpha val="50000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="lt1"/>
               </a:solidFill>
-              <a:ln w="9525">
+              <a:ln w="15875">
                 <a:solidFill>
-                  <a:schemeClr val="bg1">
-                    <a:lumMod val="65000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="accent1"/>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="fr-FR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:xVal>
             <c:numRef>
               <c:f>Burndown!$E$2:$J$2</c:f>
@@ -383,13 +438,13 @@
                   <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -419,10 +474,10 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="9525" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="bg1">
-                  <a:lumMod val="65000"/>
+                <a:schemeClr val="accent2">
+                  <a:alpha val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -432,6 +487,64 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="fr-FR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:xVal>
             <c:numRef>
               <c:f>Burndown!$E$2:$J$2</c:f>
@@ -494,8 +607,9 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -511,6 +625,50 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -519,9 +677,10 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
+              <a:schemeClr val="dk1">
                 <a:lumMod val="15000"/>
                 <a:lumOff val="85000"/>
+                <a:alpha val="54000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -535,7 +694,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
+                  <a:schemeClr val="dk1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
@@ -559,14 +718,65 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
-            <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+                <a:alpha val="54000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -577,7 +787,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
+                  <a:schemeClr val="dk1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
@@ -595,7 +805,17 @@
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
-        <a:noFill/>
+        <a:pattFill prst="ltDnDiag">
+          <a:fgClr>
+            <a:schemeClr val="dk1">
+              <a:lumMod val="15000"/>
+              <a:lumOff val="85000"/>
+            </a:schemeClr>
+          </a:fgClr>
+          <a:bgClr>
+            <a:schemeClr val="lt1"/>
+          </a:bgClr>
+        </a:pattFill>
         <a:ln>
           <a:noFill/>
         </a:ln>
@@ -608,11 +828,11 @@
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="bg1"/>
+      <a:schemeClr val="lt1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
+        <a:schemeClr val="dk1">
           <a:lumMod val="15000"/>
           <a:lumOff val="85000"/>
         </a:schemeClr>
@@ -680,25 +900,25 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="250">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
@@ -706,7 +926,31 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -715,36 +959,13 @@
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="75000"/>
         <a:lumOff val="25000"/>
       </a:schemeClr>
@@ -781,12 +1002,12 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -796,12 +1017,12 @@
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -813,15 +1034,17 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
+    <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
-          <a:schemeClr val="phClr"/>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
@@ -831,33 +1054,34 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="phClr"/>
+        <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="15875">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -873,16 +1097,15 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -890,7 +1113,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="800" kern="1200"/>
   </cs:dataTable>
   <cs:downBar>
     <cs:lnRef idx="0"/>
@@ -902,17 +1125,18 @@
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -921,12 +1145,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
@@ -940,14 +1164,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -959,13 +1183,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
     </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
@@ -973,12 +1204,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -992,14 +1223,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1011,14 +1242,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1030,12 +1261,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
@@ -1049,39 +1280,69 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
   </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea3D>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:plotArea3D>
   <cs:seriesAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -1089,12 +1350,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
@@ -1107,13 +1368,13 @@
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -1122,14 +1383,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -1138,7 +1398,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
@@ -1156,13 +1416,14 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -1171,11 +1432,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -1183,13 +1456,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
     </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
@@ -1262,16 +1542,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>25978</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>216478</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>1270000</xdr:rowOff>
+      <xdr:rowOff>1269999</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>366280</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>142587</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>562842</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>173181</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1304,8 +1584,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>202046</xdr:colOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>57727</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>1276190</xdr:rowOff>
     </xdr:to>
@@ -1331,7 +1611,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="404091" y="0"/>
-          <a:ext cx="15745114" cy="1276190"/>
+          <a:ext cx="17419204" cy="1276190"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1661,7 +1941,7 @@
   <dimension ref="B1:J24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1724,7 +2004,7 @@
       </c>
       <c r="G3" s="1">
         <f>IF(SUM(Table1[[Day 2]:[Day 5]])=0,#N/A,$E3-SUM(Table1[[Day 1]:[Day 2]]))</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H3" s="1">
         <f>IF(SUM(Table1[[Day 3]:[Day 5]])=0,#N/A,$E3-SUM(Table1[[Day 1]:[Day 3]]))</f>
@@ -1732,7 +2012,7 @@
       </c>
       <c r="I3" s="1">
         <f>IF(SUM(Table1[[Day 4]:[Day 5]])=0,#N/A,$E3-SUM(Table1[[Day 1]:[Day 4]]))</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J3" s="1">
         <f>IF(SUM(Table1[[Day 5]:[Day 5]])=0,#N/A,$E3-SUM(Table1[[Day 1]:[Day 5]]))</f>
@@ -1820,13 +2100,13 @@
         <v>1</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
       <c r="I7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J7">
         <v>1</v>
@@ -1846,13 +2126,13 @@
         <v>10</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -2052,7 +2332,7 @@
         <v>0</v>
       </c>
       <c r="G15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H15">
         <v>0</v>
@@ -2061,7 +2341,7 @@
         <v>0</v>
       </c>
       <c r="J15">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
@@ -2129,6 +2409,9 @@
       <c r="C18">
         <v>12</v>
       </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
       <c r="E18" t="s">
         <v>4</v>
       </c>
@@ -2304,19 +2587,19 @@
         <v>10</v>
       </c>
       <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
         <v>1</v>
-      </c>
-      <c r="G24">
-        <v>0</v>
-      </c>
-      <c r="H24">
-        <v>0</v>
-      </c>
-      <c r="I24">
-        <v>0</v>
-      </c>
-      <c r="J24">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>